<commit_message>
Add jaffle shop excel
</commit_message>
<xml_diff>
--- a/dbt_project/seeds/jaffle_shop.xlsx
+++ b/dbt_project/seeds/jaffle_shop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cor/github/godatadriven/dbt-excel/dbt_project/seeds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9D8E155-5C5A-384F-BF7A-BB1455A090A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5FDD42-47C7-2643-A169-A76AC5E560AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="2" xr2:uid="{998D270E-3D16-A345-80C3-503822CA5B8B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{998D270E-3D16-A345-80C3-503822CA5B8B}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_customer" sheetId="1" r:id="rId1"/>
@@ -740,7 +740,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C192FE5-E4CE-AA47-86E1-82F9ECC702BD}">
   <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -3281,7 +3281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2861AD9A-DC60-E942-ABCB-E8BE63D709DD}">
   <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>